<commit_message>
Nuevo codigo por provincias
</commit_message>
<xml_diff>
--- a/data_para_politicas.xlsx
+++ b/data_para_politicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{519D0D20-799A-414D-94DF-2BABE78DFF32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC936F36-DBB3-489C-B75F-69287739D322}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECAE09CE-A0FF-4DFB-9085-E3AEDFF0D8EF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>total</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>resto</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>st</t>
   </si>
 </sst>
 </file>
@@ -394,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EBF945-20BD-4066-A3C0-CE3E3334D1E8}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,10 +419,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>34</v>
       </c>
@@ -427,10 +439,17 @@
         <v>2</v>
       </c>
       <c r="D19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <f>+A19-SUM(B19:E19)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>112</v>
       </c>
@@ -441,10 +460,17 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F29" si="0">+A21-SUM(B21:E21)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>202</v>
       </c>
@@ -455,10 +481,17 @@
         <v>8</v>
       </c>
       <c r="D22">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="E22">
+        <v>29</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>245</v>
       </c>
@@ -469,10 +502,17 @@
         <v>17</v>
       </c>
       <c r="D23">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>312</v>
       </c>
@@ -483,10 +523,17 @@
         <v>29</v>
       </c>
       <c r="D24">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>44</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>392</v>
       </c>
@@ -497,10 +544,17 @@
         <v>29</v>
       </c>
       <c r="D25">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E25">
+        <v>53</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>488</v>
       </c>
@@ -511,10 +565,17 @@
         <v>43</v>
       </c>
       <c r="D26">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <v>57</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>581</v>
       </c>
@@ -525,10 +586,17 @@
         <v>59</v>
       </c>
       <c r="D27">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="E27">
+        <v>66</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>719</v>
       </c>
@@ -539,10 +607,17 @@
         <v>65</v>
       </c>
       <c r="D28">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="E28">
+        <v>90</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>859</v>
       </c>
@@ -553,7 +628,14 @@
         <v>83</v>
       </c>
       <c r="D29">
-        <v>400</v>
+        <v>101</v>
+      </c>
+      <c r="E29">
+        <v>97</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codigos nuevos y actualizados, datos actualizados
</commit_message>
<xml_diff>
--- a/data_para_politicas.xlsx
+++ b/data_para_politicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC936F36-DBB3-489C-B75F-69287739D322}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F40D74-2065-4515-8BE1-201307B51BC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECAE09CE-A0FF-4DFB-9085-E3AEDFF0D8EF}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EBF945-20BD-4066-A3C0-CE3E3334D1E8}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,6 +638,27 @@
         <v>202</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>901</v>
+      </c>
+      <c r="B30">
+        <v>381</v>
+      </c>
+      <c r="C30">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>106</v>
+      </c>
+      <c r="E30">
+        <v>97</v>
+      </c>
+      <c r="F30">
+        <f>+A30-SUM(B30:E30)</f>
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actuazalicion con boletin de hoy
</commit_message>
<xml_diff>
--- a/data_para_politicas.xlsx
+++ b/data_para_politicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F40D74-2065-4515-8BE1-201307B51BC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B07BA-2208-46A8-8E92-2E69CADDC09C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ECAE09CE-A0FF-4DFB-9085-E3AEDFF0D8EF}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EBF945-20BD-4066-A3C0-CE3E3334D1E8}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,6 +659,27 @@
         <v>227</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1109</v>
+      </c>
+      <c r="B31">
+        <v>462</v>
+      </c>
+      <c r="C31">
+        <v>94</v>
+      </c>
+      <c r="D31">
+        <v>145</v>
+      </c>
+      <c r="E31">
+        <v>122</v>
+      </c>
+      <c r="F31">
+        <f>+A31-SUM(B31:E31)</f>
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>